<commit_message>
Correct error in MTG tree1l + add computation oif variables for density analyses
</commit_message>
<xml_diff>
--- a/0-data/0-raw/tree1l.xlsx
+++ b/0-data/0-raw/tree1l.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohamed\Desktop\terrain_mesures_millan2020\arbres_mtg\arbre1\arbre1B\Arbre1B\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cirad.fr\AMAP - FSPM - Analyses\Allometries\0-data\0-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Arbre1B" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="98">
   <si>
     <t>CODE:</t>
   </si>
@@ -278,9 +278,6 @@
     <t>^&lt;S34</t>
   </si>
   <si>
-    <t>/A2</t>
-  </si>
-  <si>
     <t>+A5</t>
   </si>
   <si>
@@ -326,7 +323,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -394,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -432,6 +429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S666"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -786,7 +784,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -965,7 +963,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
@@ -973,7 +971,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
@@ -981,7 +979,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
@@ -989,7 +987,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B29" t="s">
         <v>27</v>
@@ -997,7 +995,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
         <v>27</v>
@@ -1028,24 +1026,24 @@
         <v>36</v>
       </c>
       <c r="O33" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="P33" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q33" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="P33" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q33" s="14" t="s">
+      <c r="R33" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="S33" s="14" t="s">
         <v>94</v>
-      </c>
-      <c r="R33" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="S33" s="14" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
@@ -1083,8 +1081,8 @@
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="C37" s="3" t="s">
-        <v>84</v>
+      <c r="C37" s="19" t="s">
+        <v>39</v>
       </c>
       <c r="N37">
         <v>455</v>
@@ -1101,7 +1099,7 @@
         <v>26.4</v>
       </c>
       <c r="M38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N38">
         <v>456</v>
@@ -1627,7 +1625,7 @@
     </row>
     <row r="79" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F79" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J79" s="15"/>
       <c r="K79" s="15"/>
@@ -1665,7 +1663,7 @@
     </row>
     <row r="82" spans="4:14" x14ac:dyDescent="0.3">
       <c r="F82" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J82" s="15"/>
       <c r="K82" s="15"/>
@@ -1781,7 +1779,7 @@
     </row>
     <row r="91" spans="4:14" x14ac:dyDescent="0.3">
       <c r="F91" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J91" s="15"/>
       <c r="K91" s="15"/>
@@ -2049,7 +2047,7 @@
     </row>
     <row r="112" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F112" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J112" s="15"/>
       <c r="K112" s="15"/>
@@ -2087,7 +2085,7 @@
     </row>
     <row r="115" spans="4:14" x14ac:dyDescent="0.3">
       <c r="F115" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J115" s="15"/>
       <c r="K115" s="15"/>
@@ -2163,7 +2161,7 @@
     </row>
     <row r="121" spans="4:14" x14ac:dyDescent="0.3">
       <c r="F121" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J121" s="15"/>
       <c r="K121" s="15"/>
@@ -2201,7 +2199,7 @@
     </row>
     <row r="124" spans="4:14" x14ac:dyDescent="0.3">
       <c r="F124" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J124" s="15"/>
       <c r="K124" s="15"/>
@@ -2391,7 +2389,7 @@
     </row>
     <row r="139" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F139" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J139" s="15"/>
       <c r="K139" s="15"/>
@@ -2429,7 +2427,7 @@
     </row>
     <row r="142" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F142" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J142" s="15"/>
       <c r="K142" s="15"/>
@@ -2581,7 +2579,7 @@
     </row>
     <row r="154" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F154" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J154" s="15"/>
       <c r="K154" s="15"/>
@@ -2605,7 +2603,7 @@
     </row>
     <row r="156" spans="3:14" x14ac:dyDescent="0.3">
       <c r="G156" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J156" s="15"/>
       <c r="K156" s="15"/>
@@ -2657,7 +2655,7 @@
     </row>
     <row r="160" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F160" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J160" s="15"/>
       <c r="K160" s="15"/>
@@ -2733,7 +2731,7 @@
     </row>
     <row r="166" spans="4:14" x14ac:dyDescent="0.3">
       <c r="F166" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J166" s="15"/>
       <c r="K166" s="15"/>
@@ -2771,7 +2769,7 @@
     </row>
     <row r="169" spans="4:14" x14ac:dyDescent="0.3">
       <c r="F169" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J169" s="15"/>
       <c r="K169" s="15"/>
@@ -2795,7 +2793,7 @@
     </row>
     <row r="171" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G171" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J171" s="15"/>
       <c r="K171" s="15"/>
@@ -2833,7 +2831,7 @@
     </row>
     <row r="174" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G174" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J174" s="15"/>
       <c r="K174" s="15"/>
@@ -2923,7 +2921,7 @@
     </row>
     <row r="181" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F181" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J181" s="15"/>
       <c r="K181" s="15"/>
@@ -2961,7 +2959,7 @@
     </row>
     <row r="184" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F184" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J184" s="15"/>
       <c r="K184" s="15"/>
@@ -7507,7 +7505,7 @@
         <v>13.95</v>
       </c>
       <c r="M466" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N466">
         <v>450</v>
@@ -8426,7 +8424,7 @@
         <v>11.77</v>
       </c>
       <c r="M519" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N519">
         <v>48</v>
@@ -9401,7 +9399,7 @@
         <v>8.15</v>
       </c>
       <c r="M578" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N578">
         <v>107</v>
@@ -10406,7 +10404,7 @@
         <v>11.1</v>
       </c>
       <c r="M639" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N639">
         <v>168</v>
@@ -10954,6 +10952,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D817E2E441AD8840AD152F485CF91FFD" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="9bd92fc451d28d7a43c1e2d68c8f297e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f3bb3ef3-874e-4bfe-a810-81c575a8e62c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6122410798bbeb3d5138414ef9c1dd21" ns2:_="">
     <xsd:import namespace="f3bb3ef3-874e-4bfe-a810-81c575a8e62c"/>
@@ -11085,15 +11092,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -11101,13 +11099,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3B9E15A-388E-4EC3-B458-5940D8058394}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{757186B9-A2D3-44A8-8412-A05B39197681}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{757186B9-A2D3-44A8-8412-A05B39197681}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3B9E15A-388E-4EC3-B458-5940D8058394}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f3bb3ef3-874e-4bfe-a810-81c575a8e62c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{210137FA-64FA-4EED-A8FE-8D505845F9D0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{210137FA-64FA-4EED-A8FE-8D505845F9D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix issues in raw mtg files + add new variable segment_index_on_axis
</commit_message>
<xml_diff>
--- a/0-data/0-raw/tree1l.xlsx
+++ b/0-data/0-raw/tree1l.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="94">
   <si>
     <t>CODE:</t>
   </si>
@@ -209,9 +209,6 @@
     <t>^&lt;S18</t>
   </si>
   <si>
-    <t>2008-2009</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -219,15 +216,6 @@
   </si>
   <si>
     <t>+A4b</t>
-  </si>
-  <si>
-    <t>2013-2014</t>
-  </si>
-  <si>
-    <t>2014-2015</t>
-  </si>
-  <si>
-    <t>2017-2018</t>
   </si>
   <si>
     <t>^&lt;S19</t>
@@ -712,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S666"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A640" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L664" sqref="L664"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,7 +772,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -963,7 +951,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
@@ -971,7 +959,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
@@ -979,7 +967,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
@@ -987,7 +975,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B29" t="s">
         <v>27</v>
@@ -995,7 +983,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B30" t="s">
         <v>27</v>
@@ -1026,24 +1014,24 @@
         <v>36</v>
       </c>
       <c r="O33" s="14" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="P33" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="Q33" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="R33" s="14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="S33" s="14" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
@@ -1099,7 +1087,7 @@
         <v>26.4</v>
       </c>
       <c r="M38" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="N38">
         <v>456</v>
@@ -1625,7 +1613,7 @@
     </row>
     <row r="79" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F79" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J79" s="15"/>
       <c r="K79" s="15"/>
@@ -1663,7 +1651,7 @@
     </row>
     <row r="82" spans="4:14" x14ac:dyDescent="0.3">
       <c r="F82" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J82" s="15"/>
       <c r="K82" s="15"/>
@@ -1779,7 +1767,7 @@
     </row>
     <row r="91" spans="4:14" x14ac:dyDescent="0.3">
       <c r="F91" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J91" s="15"/>
       <c r="K91" s="15"/>
@@ -2047,7 +2035,7 @@
     </row>
     <row r="112" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F112" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J112" s="15"/>
       <c r="K112" s="15"/>
@@ -2085,7 +2073,7 @@
     </row>
     <row r="115" spans="4:14" x14ac:dyDescent="0.3">
       <c r="F115" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J115" s="15"/>
       <c r="K115" s="15"/>
@@ -2161,7 +2149,7 @@
     </row>
     <row r="121" spans="4:14" x14ac:dyDescent="0.3">
       <c r="F121" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J121" s="15"/>
       <c r="K121" s="15"/>
@@ -2199,7 +2187,7 @@
     </row>
     <row r="124" spans="4:14" x14ac:dyDescent="0.3">
       <c r="F124" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J124" s="15"/>
       <c r="K124" s="15"/>
@@ -2389,7 +2377,7 @@
     </row>
     <row r="139" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F139" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J139" s="15"/>
       <c r="K139" s="15"/>
@@ -2427,7 +2415,7 @@
     </row>
     <row r="142" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F142" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J142" s="15"/>
       <c r="K142" s="15"/>
@@ -2579,7 +2567,7 @@
     </row>
     <row r="154" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F154" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J154" s="15"/>
       <c r="K154" s="15"/>
@@ -2603,7 +2591,7 @@
     </row>
     <row r="156" spans="3:14" x14ac:dyDescent="0.3">
       <c r="G156" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="J156" s="15"/>
       <c r="K156" s="15"/>
@@ -2655,7 +2643,7 @@
     </row>
     <row r="160" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F160" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J160" s="15"/>
       <c r="K160" s="15"/>
@@ -2731,7 +2719,7 @@
     </row>
     <row r="166" spans="4:14" x14ac:dyDescent="0.3">
       <c r="F166" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J166" s="15"/>
       <c r="K166" s="15"/>
@@ -2769,7 +2757,7 @@
     </row>
     <row r="169" spans="4:14" x14ac:dyDescent="0.3">
       <c r="F169" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J169" s="15"/>
       <c r="K169" s="15"/>
@@ -2793,7 +2781,7 @@
     </row>
     <row r="171" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G171" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="J171" s="15"/>
       <c r="K171" s="15"/>
@@ -2831,7 +2819,7 @@
     </row>
     <row r="174" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G174" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="J174" s="15"/>
       <c r="K174" s="15"/>
@@ -2921,7 +2909,7 @@
     </row>
     <row r="181" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F181" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J181" s="15"/>
       <c r="K181" s="15"/>
@@ -2959,7 +2947,7 @@
     </row>
     <row r="184" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F184" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J184" s="15"/>
       <c r="K184" s="15"/>
@@ -7499,13 +7487,13 @@
       <c r="H466" s="8"/>
       <c r="I466" s="8"/>
       <c r="J466" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K466" s="15">
         <v>13.95</v>
       </c>
       <c r="M466" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N466">
         <v>450</v>
@@ -7642,8 +7630,8 @@
       <c r="K473" s="16">
         <v>35.6</v>
       </c>
-      <c r="L473" s="9" t="s">
-        <v>61</v>
+      <c r="L473" s="9">
+        <v>2008</v>
       </c>
       <c r="N473" s="2">
         <v>2</v>
@@ -7663,7 +7651,7 @@
     </row>
     <row r="474" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B474" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J474" s="9">
         <v>2</v>
@@ -8000,7 +7988,7 @@
     </row>
     <row r="495" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B495" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J495" s="9">
         <v>28</v>
@@ -8154,7 +8142,7 @@
     </row>
     <row r="505" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B505" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E505" s="8"/>
       <c r="F505" s="8"/>
@@ -8330,7 +8318,7 @@
     </row>
     <row r="514" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B514" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E514" s="8"/>
       <c r="F514" s="8"/>
@@ -8418,13 +8406,13 @@
         <v>40</v>
       </c>
       <c r="J519" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K519" s="9">
         <v>11.77</v>
       </c>
       <c r="M519" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="N519">
         <v>48</v>
@@ -8432,7 +8420,7 @@
     </row>
     <row r="520" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B520" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J520" s="9">
         <v>10.199999999999999</v>
@@ -8883,7 +8871,7 @@
     </row>
     <row r="550" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B550" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E550" s="8"/>
       <c r="F550" s="8"/>
@@ -9358,7 +9346,7 @@
     </row>
     <row r="576" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B576" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J576" s="17"/>
       <c r="K576" s="17"/>
@@ -9393,13 +9381,13 @@
         <v>38</v>
       </c>
       <c r="J578" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K578" s="15">
         <v>8.15</v>
       </c>
       <c r="M578" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="N578">
         <v>107</v>
@@ -9407,7 +9395,7 @@
     </row>
     <row r="579" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B579" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="N579">
         <v>108</v>
@@ -9798,7 +9786,7 @@
     </row>
     <row r="600" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B600" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E600" s="8"/>
       <c r="F600" s="8"/>
@@ -9885,7 +9873,7 @@
     </row>
     <row r="605" spans="2:19" x14ac:dyDescent="0.3">
       <c r="E605" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J605" s="15"/>
       <c r="K605" s="15"/>
@@ -9909,7 +9897,7 @@
     </row>
     <row r="607" spans="2:19" x14ac:dyDescent="0.3">
       <c r="E607" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J607" s="15"/>
       <c r="K607" s="15"/>
@@ -10008,7 +9996,7 @@
     </row>
     <row r="614" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B614" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E614" s="8"/>
       <c r="F614" s="8"/>
@@ -10098,7 +10086,7 @@
     </row>
     <row r="619" spans="2:19" x14ac:dyDescent="0.3">
       <c r="E619" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F619" s="8"/>
       <c r="G619" s="8"/>
@@ -10126,7 +10114,7 @@
     </row>
     <row r="621" spans="2:19" x14ac:dyDescent="0.3">
       <c r="E621" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F621" s="8"/>
       <c r="G621" s="8"/>
@@ -10235,7 +10223,7 @@
     </row>
     <row r="628" spans="2:14" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B628" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E628" s="8"/>
       <c r="F628" s="8"/>
@@ -10398,13 +10386,13 @@
       <c r="F639" s="8"/>
       <c r="G639" s="8"/>
       <c r="J639" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K639" s="15">
         <v>11.1</v>
       </c>
       <c r="M639" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="N639">
         <v>168</v>
@@ -10442,7 +10430,7 @@
     </row>
     <row r="642" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B642" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E642" s="8"/>
       <c r="F642" s="8"/>
@@ -10453,8 +10441,8 @@
       <c r="K642" s="9">
         <v>15.24</v>
       </c>
-      <c r="L642" s="9" t="s">
-        <v>65</v>
+      <c r="L642" s="9">
+        <v>2013</v>
       </c>
       <c r="N642" s="2">
         <v>171</v>
@@ -10632,7 +10620,7 @@
     </row>
     <row r="651" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B651" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E651" s="8"/>
       <c r="F651" s="8"/>
@@ -10643,8 +10631,8 @@
       <c r="K651" s="9">
         <v>13.3</v>
       </c>
-      <c r="L651" s="9" t="s">
-        <v>66</v>
+      <c r="L651" s="9">
+        <v>2014</v>
       </c>
       <c r="N651" s="2">
         <v>180</v>
@@ -10816,7 +10804,7 @@
     </row>
     <row r="660" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B660" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J660" s="9">
         <v>5.8</v>
@@ -10867,7 +10855,7 @@
     </row>
     <row r="663" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B663" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J663" s="9">
         <v>18.5</v>
@@ -10875,8 +10863,8 @@
       <c r="K663" s="9">
         <v>10.039999999999999</v>
       </c>
-      <c r="L663" s="9" t="s">
-        <v>67</v>
+      <c r="L663" s="9">
+        <v>2017</v>
       </c>
       <c r="N663" s="2">
         <v>192</v>
@@ -10918,7 +10906,7 @@
     </row>
     <row r="666" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B666" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J666" s="9">
         <v>7.4</v>
@@ -10952,15 +10940,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D817E2E441AD8840AD152F485CF91FFD" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="9bd92fc451d28d7a43c1e2d68c8f297e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f3bb3ef3-874e-4bfe-a810-81c575a8e62c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6122410798bbeb3d5138414ef9c1dd21" ns2:_="">
     <xsd:import namespace="f3bb3ef3-874e-4bfe-a810-81c575a8e62c"/>
@@ -11092,6 +11071,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -11099,14 +11087,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{757186B9-A2D3-44A8-8412-A05B39197681}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3B9E15A-388E-4EC3-B458-5940D8058394}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11124,11 +11104,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{757186B9-A2D3-44A8-8412-A05B39197681}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{210137FA-64FA-4EED-A8FE-8D505845F9D0}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="f3bb3ef3-874e-4bfe-a810-81c575a8e62c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>